<commit_message>
Add Predicates and refactor of Ball (hjHlRz1Y)
Debug scripts commenting (not fixing) to let project compile
</commit_message>
<xml_diff>
--- a/Resources/List of States and Predicates.xlsx
+++ b/Resources/List of States and Predicates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5994590E-C15B-44E9-95F2-B93993D2A0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41601A90-51EC-4463-A4D5-7C8887784269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
+    <workbookView xWindow="18351" yWindow="5777" windowWidth="14238" windowHeight="11854" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
   <si>
     <t>Athlete Class</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>To State</t>
-  </si>
-  <si>
     <t>postPointState</t>
   </si>
   <si>
@@ -87,16 +78,130 @@
   </si>
   <si>
     <t>OnBallHitGround</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>groundState</t>
+  </si>
+  <si>
+    <t>heldState</t>
+  </si>
+  <si>
+    <t>OnBallGiven</t>
+  </si>
+  <si>
+    <t>inFlightState</t>
+  </si>
+  <si>
+    <t>OnTargetSet</t>
+  </si>
+  <si>
+    <t>pos == targetPos || pos.y &lt;= 0</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>ServePosState</t>
+  </si>
+  <si>
+    <t>team serving &amp; athlete serving</t>
+  </si>
+  <si>
+    <t>team serving &amp; !athlete serving</t>
+  </si>
+  <si>
+    <t>NonServeState</t>
+  </si>
+  <si>
+    <t>ReceiveServeState</t>
+  </si>
+  <si>
+    <t>!team serving</t>
+  </si>
+  <si>
+    <t>DefenseState</t>
+  </si>
+  <si>
+    <t>OnBallServed</t>
+  </si>
+  <si>
+    <t>DigReadyState</t>
+  </si>
+  <si>
+    <t>MyBall &amp; JudgeInBounds</t>
+  </si>
+  <si>
+    <t>OffenseState</t>
+  </si>
+  <si>
+    <t>!MyBall</t>
+  </si>
+  <si>
+    <t>DefenseBlockerState</t>
+  </si>
+  <si>
+    <t>DefenseDefenderState</t>
+  </si>
+  <si>
+    <t>PosType = Blocker</t>
+  </si>
+  <si>
+    <t>PosType = Defender</t>
+  </si>
+  <si>
+    <t>OnBodyTrigger &amp; HitsForTeam = 0</t>
+  </si>
+  <si>
+    <t>OnBodyTrigger &amp; HitsForTeam IN(1,2)</t>
+  </si>
+  <si>
+    <t>OnSpikeTrigger</t>
+  </si>
+  <si>
+    <t>OnTargetSet &amp; TargetPos.x != ai.CourtSide</t>
+  </si>
+  <si>
+    <t>OnTargetSet &amp; TargetPos.x == ai.CourtSide</t>
+  </si>
+  <si>
+    <t>delay timer &amp; stopped [event]</t>
+  </si>
+  <si>
+    <t>delay timer [event]</t>
+  </si>
+  <si>
+    <t>OnTargetSet &amp; TargetPos.x == ai.CourtSide &amp; possession == courtside</t>
+  </si>
+  <si>
+    <t>OnTargetSet &amp; TargetPos.x == ai.CourtSide &amp; JudgeInBounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,12 +227,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,11 +572,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C076F8-7A7E-40D4-88D6-6233B17A6EB3}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -483,108 +591,424 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor MatchManager StateMachine (MSYXoY06)
This includes updating the Excel's list of states and predicates.
Also pass current profile's current state directly from state machine.
</commit_message>
<xml_diff>
--- a/Resources/List of States and Predicates.xlsx
+++ b/Resources/List of States and Predicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41601A90-51EC-4463-A4D5-7C8887784269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C1DAA-A851-4C38-B461-DCC42B948DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18351" yWindow="5777" windowWidth="14238" windowHeight="11854" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
-  <si>
-    <t>Athlete Class</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
   <si>
     <t>Player</t>
   </si>
@@ -186,13 +183,55 @@
   </si>
   <si>
     <t>OnTargetSet &amp; TargetPos.x == ai.CourtSide &amp; JudgeInBounds</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>MatchStartState</t>
+  </si>
+  <si>
+    <t>PrePointState</t>
+  </si>
+  <si>
+    <t>OnInteract</t>
+  </si>
+  <si>
+    <t>InPlayState</t>
+  </si>
+  <si>
+    <t>MatchEndState</t>
+  </si>
+  <si>
+    <t>GameEnd == true</t>
+  </si>
+  <si>
+    <t>timeUntilChange [event]</t>
+  </si>
+  <si>
+    <t>MatchInfo.Initialize() [event]</t>
+  </si>
+  <si>
+    <t>PauseState</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>OnPause</t>
+  </si>
+  <si>
+    <t>OnUnPause</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +241,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -237,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C076F8-7A7E-40D4-88D6-6233B17A6EB3}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -588,427 +638,550 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>44</v>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update for Use Predicates in State Machine (hjHlRz1Y)
- Updated Game test scene
- Athlete update to use new StateMachine, removed logging for adjusting position towards ball, removed ball variable because the collision has been handled by the CollisionTriggerReporter
- Player using new StateMachine with Predicates
- Update to AthleteStateMonitor to use StateChanged from the StateMachine [stale]
- List of States and Predicates log updated for more detail of missing events
</commit_message>
<xml_diff>
--- a/Resources/List of States and Predicates.xlsx
+++ b/Resources/List of States and Predicates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C1DAA-A851-4C38-B461-DCC42B948DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77C5027-B0FF-4A36-8898-F7F3873FC76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
+    <workbookView xWindow="16671" yWindow="4706" windowWidth="14238" windowHeight="11854" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,21 +113,12 @@
     <t>ServePosState</t>
   </si>
   <si>
-    <t>team serving &amp; athlete serving</t>
-  </si>
-  <si>
-    <t>team serving &amp; !athlete serving</t>
-  </si>
-  <si>
     <t>NonServeState</t>
   </si>
   <si>
     <t>ReceiveServeState</t>
   </si>
   <si>
-    <t>!team serving</t>
-  </si>
-  <si>
     <t>DefenseState</t>
   </si>
   <si>
@@ -225,6 +216,15 @@
   </si>
   <si>
     <t>OnUnPause</t>
+  </si>
+  <si>
+    <t>TransitionToServeState [event] team serving &amp; athlete serving</t>
+  </si>
+  <si>
+    <t>TransitionToServeState [event] team serving &amp; !athlete serving</t>
+  </si>
+  <si>
+    <t>TransitionToServeState [event] !team serving</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -638,7 +638,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -820,7 +820,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -831,10 +831,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -845,10 +845,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -862,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -870,13 +870,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -884,13 +884,13 @@
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -898,13 +898,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -915,10 +915,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -926,13 +926,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -940,13 +940,13 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -954,13 +954,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -968,13 +968,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -982,13 +982,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -996,13 +996,13 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1010,13 +1010,13 @@
         <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1024,13 +1024,13 @@
         <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1038,13 +1038,13 @@
         <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1052,21 +1052,21 @@
         <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>2</v>
@@ -1074,52 +1074,52 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>1</v>
@@ -1130,58 +1130,58 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on Blocker AI
</commit_message>
<xml_diff>
--- a/Resources/List of States and Predicates.xlsx
+++ b/Resources/List of States and Predicates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77C5027-B0FF-4A36-8898-F7F3873FC76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014DBD09-1C5A-4A02-A3B2-3BB763C5FE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16671" yWindow="4706" windowWidth="14238" windowHeight="11854" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{B078746C-A2D3-43CC-9781-16A37D062287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="65">
   <si>
     <t>Player</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>TransitionToServeState [event] !team serving</t>
+  </si>
+  <si>
+    <t>AI Blocker</t>
+  </si>
+  <si>
+    <t>wait, is there any other?</t>
   </si>
 </sst>
 </file>
@@ -622,11 +628,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C076F8-7A7E-40D4-88D6-6233B17A6EB3}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1184,6 +1190,17 @@
         <v>59</v>
       </c>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>